<commit_message>
commit code release v1
</commit_message>
<xml_diff>
--- a/TraiNghiemSangTao/TraiNghiemSangTao/Utils/Files/ds-noidungkhac.xlsx
+++ b/TraiNghiemSangTao/TraiNghiemSangTao/Utils/Files/ds-noidungkhac.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>DANH SÁCH NỘI DUNG KHÁC</t>
   </si>
   <si>
-    <t>Từ ngày 01/07/2018 tới ngày 20/08/2018</t>
+    <t>Từ ngày 22/07/2018 tới ngày 22/08/2018</t>
   </si>
   <si>
     <t>STT</t>
@@ -68,22 +68,22 @@
     <t>Lớp 1</t>
   </si>
   <si>
-    <t>11/07/2018</t>
+    <t>24/07/2018</t>
   </si>
   <si>
     <t>abc</t>
   </si>
   <si>
-    <t>dsadwa</t>
-  </si>
-  <si>
-    <t>dwasdwada</t>
+    <t xml:space="preserve">ssd </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sad </t>
   </si>
   <si>
     <t>Tỉnh An Giang</t>
   </si>
   <si>
-    <t>Tin học, Kĩ thuật, Âm nhạc, Giáo trình Tiểu học</t>
+    <t>Vật lí, Tin học, Tiếng Việt, Âm nhạc</t>
   </si>
   <si>
     <t>Thành Trương Hữu</t>
@@ -99,18 +99,6 @@
   </si>
   <si>
     <t>08/07/2018</t>
-  </si>
-  <si>
-    <t>24/07/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssd </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sad </t>
-  </si>
-  <si>
-    <t>Vật lí, Tin học, Tiếng Việt, Âm nhạc</t>
   </si>
   <si>
     <t>25/07/2018</t>
@@ -246,7 +234,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:P12"/>
+  <dimension ref="A2:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -405,14 +393,17 @@
       <c r="C8" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="D8" s="0">
+        <v>100</v>
+      </c>
       <c r="E8" s="0" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>31</v>
@@ -424,19 +415,19 @@
         <v>32</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9">
@@ -450,40 +441,40 @@
         <v>17</v>
       </c>
       <c r="D9" s="0">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
@@ -500,25 +491,25 @@
         <v>21</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>22</v>
       </c>
       <c r="J10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="M10" s="0" t="s">
         <v>25</v>
@@ -530,7 +521,7 @@
         <v>27</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -547,25 +538,25 @@
         <v>21</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>19</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>22</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="M11" s="0" t="s">
         <v>25</v>
@@ -577,53 +568,6 @@
         <v>27</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0">
-        <v>6</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="0">
-        <v>21</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="O12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="P12" s="0" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>